<commit_message>
changes to log reg in r
</commit_message>
<xml_diff>
--- a/results/LOG_REG.xlsx
+++ b/results/LOG_REG.xlsx
@@ -1,33 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\João Matos\Documents\Education\MIT\Projects\Race Disparities in Sepsis\mit-tmle\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tristan/Documents/Projekte/Boston Celi/1 Causal Inference/Race Interventions/mit-tmle/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{691B479B-B220-4241-ABE0-88877B86CBA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08823977-07AA-764D-BB13-2E0216ADCED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MIMIC" sheetId="1" r:id="rId1"/>
     <sheet name="eICU" sheetId="2" r:id="rId2"/>
-    <sheet name="processed" sheetId="3" r:id="rId3"/>
+    <sheet name="comb" sheetId="4" r:id="rId3"/>
+    <sheet name="processed" sheetId="3" r:id="rId4"/>
+    <sheet name="proc_comb" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="33">
   <si>
     <t>SOFA</t>
   </si>
@@ -132,13 +131,16 @@
   <si>
     <t>Odds Ratio (CI)
  White vs. Non-White</t>
+  </si>
+  <si>
+    <t>Comb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -165,6 +167,17 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -174,7 +187,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -182,24 +195,56 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -212,33 +257,56 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="6" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -554,14 +622,14 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="8" max="20" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="20" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.5" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="6.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -577,29 +645,29 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="4" t="s">
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="4" t="s">
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -661,7 +729,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -726,7 +794,7 @@
         <v>0.6996862226198759</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -791,7 +859,7 @@
         <v>0.14604122647145779</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -856,7 +924,7 @@
         <v>3.352209659919215</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -878,16 +946,16 @@
       <c r="H6" s="1">
         <v>2.0303663723171089E-2</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="3">
         <v>0.15444435746675034</v>
       </c>
       <c r="J6" s="1">
         <v>2.806363139415519E-2</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="3">
         <v>0.34782715586151403</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="3">
         <v>0.88594598852589046</v>
       </c>
       <c r="M6" s="1">
@@ -902,7 +970,7 @@
       <c r="P6" s="1">
         <v>4.9379107472904568E-2</v>
       </c>
-      <c r="Q6" s="5">
+      <c r="Q6" s="3">
         <v>0.5993976831686606</v>
       </c>
       <c r="R6" s="1">
@@ -914,14 +982,14 @@
       <c r="T6" s="1">
         <v>4.3972584807742551E-12</v>
       </c>
-      <c r="U6" s="5">
+      <c r="U6" s="3">
         <v>0.38891668209609193</v>
       </c>
-      <c r="V6" s="5">
+      <c r="V6" s="3">
         <v>0.65505264725132828</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -938,7 +1006,7 @@
         <v>8.610201175008081E-26</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -955,7 +1023,7 @@
         <v>4.2178417094128644E-10</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -972,7 +1040,7 @@
         <v>2.738268689919817E-20</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -989,7 +1057,7 @@
         <v>4.9379107472904568E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1006,7 +1074,7 @@
         <v>0.5993976831686606</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1023,7 +1091,7 @@
         <v>6.0397657786188027E-21</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1040,7 +1108,7 @@
         <v>9.4801743458325452E-11</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1057,7 +1125,7 @@
         <v>4.3972584807742551E-12</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -1074,7 +1142,7 @@
         <v>0.38891668209609193</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -1106,15 +1174,15 @@
   <dimension ref="A1:V16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E15"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1130,29 +1198,29 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="4" t="s">
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="4" t="s">
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1214,7 +1282,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1275,7 +1343,7 @@
       </c>
       <c r="V3" s="1"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1336,7 +1404,7 @@
       </c>
       <c r="V4" s="1"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1397,7 +1465,7 @@
       </c>
       <c r="V5" s="1"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1450,7 +1518,7 @@
       </c>
       <c r="V6" s="1"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1467,7 +1535,7 @@
         <v>3.7614586814981702E-33</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1484,7 +1552,7 @@
         <v>3.888977497180045E-18</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1501,7 +1569,7 @@
         <v>2.9473185237582918E-18</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1518,7 +1586,7 @@
         <v>0.97851099567074218</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1535,7 +1603,7 @@
         <v>0.97531628674358151</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1552,7 +1620,7 @@
         <v>1.8060824641937391E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1569,7 +1637,7 @@
         <v>7.0274651563082564E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1586,7 +1654,7 @@
         <v>9.6554055855737893E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -1603,7 +1671,7 @@
         <v>0.3514863588822163</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -1619,217 +1687,602 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6EE9FD-E04A-1B49-B8E8-A06D1A48705F}">
+  <dimension ref="A1:V16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="15"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1.1464086253903594</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1.0522206844645743</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1.2490276571954815</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1.7859781053329708E-3</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1.1501060738118938</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1.0149126450412029</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1.3033082083289138</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2.8381832317266327E-2</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1.2003411110367985</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1.0514690835535825</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1.3702911529986346</v>
+      </c>
+      <c r="E4" s="1">
+        <v>6.8753688959064686E-3</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.8733928506005515</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.64674458637657894</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1.1794688158951114</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.377170179292666</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1.6450518443358078</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.68560235521592516</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3.9471795129705285</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.26498056312302865</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.71376953055250036</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.62208784789881533</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.81896302020032907</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1.5304637777699025E-6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.51535031698170841</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.36466030359707302</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.72831055805460876</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1.7235425397791034E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.59841644836381103</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.4906833997111138</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.72980305810872692</v>
+      </c>
+      <c r="E9" s="1">
+        <v>3.9732785637163997E-7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1.0103488835969268</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.78990668945638298</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1.2923106997461664</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.93465951555910753</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1.1148168957222486</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.68086442488967502</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1.8253512234673925</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.66571592446898264</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1.374269158888465</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1.2557498354121508</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1.5039744922221274</v>
+      </c>
+      <c r="E12" s="1">
+        <v>4.8813356808069523E-12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1.4003722921047703</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1.2260204915367277</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1.5995185806696786</v>
+      </c>
+      <c r="E13" s="1">
+        <v>6.9167180514873738E-7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1.3694723678586598</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1.1983280705820289</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1.5650593625980023</v>
+      </c>
+      <c r="E14" s="1">
+        <v>3.9071432244698876E-6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1.251969416989801</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.89492485565891888</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1.7514626073534523</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.18956365188063862</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.66073162185445655</v>
+      </c>
+      <c r="C16" s="1">
+        <v>6.7452298291336768E-2</v>
+      </c>
+      <c r="D16" s="1">
+        <v>6.4722224027537836</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.72188722968054342</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="M1:Q1"/>
+    <mergeCell ref="R1:V1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72440BF3-33B5-4D9D-850C-0A4456E13577}">
   <dimension ref="A3:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="196" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView zoomScale="196" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:7" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="6" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-    </row>
-    <row r="4" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+    </row>
+    <row r="4" spans="1:7" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:7" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="10" t="str">
+      <c r="C5" s="7" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!H3, 2), " (", ROUND(MIMIC!H4,2), " - ", ROUND(MIMIC!H5,2),  ")", IF(AND(MIMIC!H6 &lt;0.05, NOT(ISBLANK(MIMIC!H6))), "*", " ") )</f>
         <v>1.08 (1.01 - 1.15)*</v>
       </c>
-      <c r="D5" s="7" t="str">
+      <c r="D5" s="4" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!I3, 2), " (", ROUND(MIMIC!I4,2), " - ", ROUND(MIMIC!I5,2),  ")", IF(AND(MIMIC!I6 &lt;0.05, NOT(ISBLANK(MIMIC!I6))), "*", " ") )</f>
         <v xml:space="preserve">1.07 (0.97 - 1.19) </v>
       </c>
-      <c r="E5" s="10" t="str">
+      <c r="E5" s="7" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!J3, 2), " (", ROUND(MIMIC!J4,2), " - ", ROUND(MIMIC!J5,2),  ")", IF(AND(MIMIC!J6 &lt;0.05, NOT(ISBLANK(MIMIC!J6))), "*", " ") )</f>
         <v>1.12 (1.01 - 1.23)*</v>
       </c>
-      <c r="F5" s="7" t="str">
+      <c r="F5" s="4" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!K3, 2), " (", ROUND(MIMIC!K4,2), " - ", ROUND(MIMIC!K5,2),  ")", IF(AND(MIMIC!K6 &lt;0.05, NOT(ISBLANK(MIMIC!K6))), "*", " ") )</f>
         <v xml:space="preserve">0.9 (0.72 - 1.12) </v>
       </c>
-      <c r="G5" s="7" t="str">
+      <c r="G5" s="4" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!L3, 2), " (", ROUND(MIMIC!L4,2), " - ", ROUND(MIMIC!L5,2),  ")", IF(AND(MIMIC!L6 &lt;0.05, NOT(ISBLANK(MIMIC!L6))), "*", " ") )</f>
         <v xml:space="preserve">1.06 (0.48 - 2.33) </v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7" t="s">
+    <row r="6" spans="1:7" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="17"/>
+      <c r="B6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="10" t="str">
+      <c r="C6" s="7" t="str">
         <f>_xlfn.CONCAT(ROUND(eICU!H3, 2), " (", ROUND(eICU!H4,2), " - ", ROUND(eICU!H5,2),  ")", IF(AND(eICU!H6 &lt;0.05, NOT(ISBLANK(eICU!H6))), "*", " ") )</f>
         <v>1.09 (1.03 - 1.14)*</v>
       </c>
-      <c r="D6" s="7" t="str">
+      <c r="D6" s="4" t="str">
         <f>_xlfn.CONCAT(ROUND(eICU!I3, 2), " (", ROUND(eICU!I4,2), " - ", ROUND(eICU!I5,2),  ")", IF(AND(eICU!I6 &lt;0.05, NOT(ISBLANK(eICU!I6))), "*", " ") )</f>
         <v xml:space="preserve">0.99 (0.93 - 1.05) </v>
       </c>
-      <c r="E6" s="10" t="str">
+      <c r="E6" s="7" t="str">
         <f>_xlfn.CONCAT(ROUND(eICU!J3, 2), " (", ROUND(eICU!J4,2), " - ", ROUND(eICU!J5,2),  ")", IF(AND(eICU!J6 &lt;0.05, NOT(ISBLANK(eICU!J6))), "*", " ") )</f>
         <v>1.31 (1.2 - 1.43)*</v>
       </c>
-      <c r="F6" s="7" t="str">
+      <c r="F6" s="4" t="str">
         <f>_xlfn.CONCAT(ROUND(eICU!K3, 2), " (", ROUND(eICU!K4,2), " - ", ROUND(eICU!K5,2),  ")", IF(AND(eICU!K6 &lt;0.05, NOT(ISBLANK(eICU!K6))), "*", " ") )</f>
         <v xml:space="preserve">0.97 (0.72 - 1.32) </v>
       </c>
-      <c r="G6" s="7" t="str">
+      <c r="G6" s="4" t="str">
         <f>_xlfn.CONCAT(ROUND(eICU!L3, 2), " (", ROUND(eICU!L4,2), " - ", ROUND(eICU!L5,2),  ")", IF(AND(eICU!L6 &lt;0.05, NOT(ISBLANK(eICU!L6))), "*", " ") )</f>
         <v xml:space="preserve">0 (0 - 0) </v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:7" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="10" t="str">
+      <c r="C7" s="7" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!M3, 2), " (", ROUND(MIMIC!M4,2), " - ", ROUND(MIMIC!M5,2),  ")", IF(AND(MIMIC!M6 &lt;0.05, NOT(ISBLANK(MIMIC!M6))), "*", " ") )</f>
         <v>0.61 (0.55 - 0.66)*</v>
       </c>
-      <c r="D7" s="10" t="str">
+      <c r="D7" s="7" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!N3, 2), " (", ROUND(MIMIC!N4,2), " - ", ROUND(MIMIC!N5,2),  ")", IF(AND(MIMIC!N6 &lt;0.05, NOT(ISBLANK(MIMIC!N6))), "*", " ") )</f>
         <v>0.5 (0.4 - 0.62)*</v>
       </c>
-      <c r="E7" s="10" t="str">
+      <c r="E7" s="7" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!O3, 2), " (", ROUND(MIMIC!O4,2), " - ", ROUND(MIMIC!O5,2),  ")", IF(AND(MIMIC!O6 &lt;0.05, NOT(ISBLANK(MIMIC!O6))), "*", " ") )</f>
         <v>0.53 (0.47 - 0.61)*</v>
       </c>
-      <c r="F7" s="10" t="str">
+      <c r="F7" s="7" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!P3, 2), " (", ROUND(MIMIC!P4,2), " - ", ROUND(MIMIC!P5,2),  ")", IF(AND(MIMIC!P6 &lt;0.05, NOT(ISBLANK(MIMIC!P6))), "*", " ") )</f>
         <v>0.83 (0.7 - 1)*</v>
       </c>
-      <c r="G7" s="7" t="str">
+      <c r="G7" s="4" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!Q3, 2), " (", ROUND(MIMIC!Q4,2), " - ", ROUND(MIMIC!Q5,2),  ")", IF(AND(MIMIC!Q6 &lt;0.05, NOT(ISBLANK(MIMIC!Q6))), "*", " ") )</f>
         <v xml:space="preserve">1.11 (0.75 - 1.63) </v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7" t="s">
+    <row r="8" spans="1:7" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="17"/>
+      <c r="B8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="10" t="str">
+      <c r="C8" s="7" t="str">
         <f>_xlfn.CONCAT(ROUND(eICU!M3, 2), " (", ROUND(eICU!M4,2), " - ", ROUND(eICU!M5,2),  ")",, IF(AND(eICU!M6 &lt;0.05, NOT(ISBLANK(eICU!M6))), "*", " ") )</f>
         <v>0.63 (0.58 - 0.68)*</v>
       </c>
-      <c r="D8" s="10" t="str">
+      <c r="D8" s="7" t="str">
         <f>_xlfn.CONCAT(ROUND(eICU!N3, 2), " (", ROUND(eICU!N4,2), " - ", ROUND(eICU!N5,2),  ")",, IF(AND(eICU!N6 &lt;0.05, NOT(ISBLANK(eICU!N6))), "*", " ") )</f>
         <v>0.58 (0.52 - 0.66)*</v>
       </c>
-      <c r="E8" s="10" t="str">
+      <c r="E8" s="7" t="str">
         <f>_xlfn.CONCAT(ROUND(eICU!O3, 2), " (", ROUND(eICU!O4,2), " - ", ROUND(eICU!O5,2),  ")",, IF(AND(eICU!O6 &lt;0.05, NOT(ISBLANK(eICU!O6))), "*", " ") )</f>
         <v>0.62 (0.55 - 0.69)*</v>
       </c>
-      <c r="F8" s="7" t="str">
+      <c r="F8" s="4" t="str">
         <f>_xlfn.CONCAT(ROUND(eICU!P3, 2), " (", ROUND(eICU!P4,2), " - ", ROUND(eICU!P5,2),  ")",, IF(AND(eICU!P6 &lt;0.05, NOT(ISBLANK(eICU!P6))), "*", " ") )</f>
         <v xml:space="preserve">1 (0.81 - 1.25) </v>
       </c>
-      <c r="G8" s="7" t="str">
+      <c r="G8" s="4" t="str">
         <f>_xlfn.CONCAT(ROUND(eICU!Q3, 2), " (", ROUND(eICU!Q4,2), " - ", ROUND(eICU!Q5,2),  ")",, IF(AND(eICU!Q6 &lt;0.05, NOT(ISBLANK(eICU!Q6))), "*", " ") )</f>
         <v xml:space="preserve">0.99 (0.46 - 2.13) </v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:7" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="10" t="str">
+      <c r="C9" s="7" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!R3, 2), " (", ROUND(MIMIC!R4,2), " - ", ROUND(MIMIC!R5,2),  ")", IF(AND(MIMIC!R6 &lt;0.05, NOT(ISBLANK(MIMIC!R6))), "*", " ") )</f>
         <v>1.39 (1.3 - 1.49)*</v>
       </c>
-      <c r="D9" s="10" t="str">
+      <c r="D9" s="7" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!S3, 2), " (", ROUND(MIMIC!S4,2), " - ", ROUND(MIMIC!S5,2),  ")", IF(AND(MIMIC!S6 &lt;0.05, NOT(ISBLANK(MIMIC!S6))), "*", " ") )</f>
         <v>1.42 (1.27 - 1.57)*</v>
       </c>
-      <c r="E9" s="10" t="str">
+      <c r="E9" s="7" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!T3, 2), " (", ROUND(MIMIC!T4,2), " - ", ROUND(MIMIC!T5,2),  ")", IF(AND(MIMIC!T6 &lt;0.05, NOT(ISBLANK(MIMIC!T6))), "*", " ") )</f>
         <v>1.42 (1.28 - 1.56)*</v>
       </c>
-      <c r="F9" s="7" t="str">
+      <c r="F9" s="4" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!U3, 2), " (", ROUND(MIMIC!U4,2), " - ", ROUND(MIMIC!U5,2),  ")", IF(AND(MIMIC!U6 &lt;0.05, NOT(ISBLANK(MIMIC!U6))), "*", " ") )</f>
         <v xml:space="preserve">1.12 (0.87 - 1.45) </v>
       </c>
-      <c r="G9" s="7" t="str">
+      <c r="G9" s="4" t="str">
         <f>_xlfn.CONCAT(ROUND(MIMIC!V3, 2), " (", ROUND(MIMIC!V4,2), " - ", ROUND(MIMIC!V5,2),  ")", IF(AND(MIMIC!V6 &lt;0.05, NOT(ISBLANK(MIMIC!V6))), "*", " ") )</f>
         <v xml:space="preserve">0.7 (0.15 - 3.35) </v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7" t="s">
+    <row r="10" spans="1:7" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="17"/>
+      <c r="B10" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="10" t="str">
+      <c r="C10" s="7" t="str">
         <f>_xlfn.CONCAT(ROUND(eICU!R3, 2), " (", ROUND(eICU!R4,2), " - ", ROUND(eICU!R5,2),  ")",, IF(AND(eICU!R6 &lt;0.05, NOT(ISBLANK(eICU!R6))), "*", " ") )</f>
         <v>1.12 (1.06 - 1.18)*</v>
       </c>
-      <c r="D10" s="10" t="str">
+      <c r="D10" s="7" t="str">
         <f>_xlfn.CONCAT(ROUND(eICU!S3, 2), " (", ROUND(eICU!S4,2), " - ", ROUND(eICU!S5,2),  ")",, IF(AND(eICU!S6 &lt;0.05, NOT(ISBLANK(eICU!S6))), "*", " ") )</f>
         <v>1.09 (1.02 - 1.17)*</v>
       </c>
-      <c r="E10" s="10" t="str">
+      <c r="E10" s="7" t="str">
         <f>_xlfn.CONCAT(ROUND(eICU!T3, 2), " (", ROUND(eICU!T4,2), " - ", ROUND(eICU!T5,2),  ")",, IF(AND(eICU!T6 &lt;0.05, NOT(ISBLANK(eICU!T6))), "*", " ") )</f>
         <v>1.16 (1.06 - 1.27)*</v>
       </c>
-      <c r="F10" s="7" t="str">
+      <c r="F10" s="4" t="str">
         <f>_xlfn.CONCAT(ROUND(eICU!U3, 2), " (", ROUND(eICU!U4,2), " - ", ROUND(eICU!U5,2),  ")",, IF(AND(eICU!U6 &lt;0.05, NOT(ISBLANK(eICU!U6))), "*", " ") )</f>
         <v xml:space="preserve">1.18 (0.83 - 1.69) </v>
       </c>
-      <c r="G10" s="7" t="str">
+      <c r="G10" s="4" t="str">
         <f>_xlfn.CONCAT(ROUND(eICU!V3, 2), " (", ROUND(eICU!V4,2), " - ", ROUND(eICU!V5,2),  ")",, IF(AND(eICU!V6 &lt;0.05, NOT(ISBLANK(eICU!V6))), "*", " ") )</f>
         <v xml:space="preserve">0 (0 - 0) </v>
       </c>
@@ -1844,4 +2297,154 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35A21450-980D-7A4C-82EA-70868119DA27}">
+  <dimension ref="A3:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="196" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:7" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="20"/>
+      <c r="C3" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="22"/>
+    </row>
+    <row r="4" spans="1:7" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="8" t="str">
+        <f>_xlfn.CONCAT(ROUND(comb!B2, 2), " (", ROUND(comb!C2,2), " - ", ROUND(comb!D2,2),  ")", IF(OR(comb!C2 &gt;1, comb!D2 &lt;1), "*", " ") )</f>
+        <v>1.15 (1.05 - 1.25)*</v>
+      </c>
+      <c r="D5" s="8" t="str">
+        <f>_xlfn.CONCAT(ROUND(comb!B3, 2), " (", ROUND(comb!C3,2), " - ", ROUND(comb!D3,2),  ")", IF(OR(comb!C3 &gt;1, comb!D3 &lt;1), "*", " ") )</f>
+        <v>1.15 (1.01 - 1.3)*</v>
+      </c>
+      <c r="E5" s="8" t="str">
+        <f>_xlfn.CONCAT(ROUND(comb!B4, 2), " (", ROUND(comb!C4,2), " - ", ROUND(comb!D4,2),  ")", IF(OR(comb!C4 &gt;1, comb!D4 &lt;1), "*", " ") )</f>
+        <v>1.2 (1.05 - 1.37)*</v>
+      </c>
+      <c r="F5" s="8" t="str">
+        <f>_xlfn.CONCAT(ROUND(comb!B5, 2), " (", ROUND(comb!C5,2), " - ", ROUND(comb!D5,2),  ")", IF(OR(comb!C5 &gt;1, comb!D5 &lt;1), "*", " ") )</f>
+        <v xml:space="preserve">0.87 (0.65 - 1.18) </v>
+      </c>
+      <c r="G5" s="9" t="str">
+        <f>_xlfn.CONCAT(ROUND(comb!B6, 2), " (", ROUND(comb!C6,2), " - ", ROUND(comb!D6,2),  ")", IF(OR(comb!C6 &gt;1, comb!D6 &lt;1), "*", " ") )</f>
+        <v xml:space="preserve">1.65 (0.69 - 3.95) </v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="8" t="str">
+        <f>_xlfn.CONCAT(ROUND(comb!B7, 2), " (", ROUND(comb!C7,2), " - ", ROUND(comb!D7,2),  ")", IF(OR(comb!C7 &gt;1, comb!D7 &lt;1), "*", " ") )</f>
+        <v>0.71 (0.62 - 0.82)*</v>
+      </c>
+      <c r="D6" s="8" t="str">
+        <f>_xlfn.CONCAT(ROUND(comb!B8, 2), " (", ROUND(comb!C8,2), " - ", ROUND(comb!D8,2),  ")", IF(OR(comb!C8 &gt;1, comb!D8 &lt;1), "*", " ") )</f>
+        <v>0.52 (0.36 - 0.73)*</v>
+      </c>
+      <c r="E6" s="8" t="str">
+        <f>_xlfn.CONCAT(ROUND(comb!B9, 2), " (", ROUND(comb!C9,2), " - ", ROUND(comb!D9,2),  ")", IF(OR(comb!C9 &gt;1, comb!D9 &lt;1), "*", " ") )</f>
+        <v>0.6 (0.49 - 0.73)*</v>
+      </c>
+      <c r="F6" s="8" t="str">
+        <f>_xlfn.CONCAT(ROUND(comb!B10, 2), " (", ROUND(comb!C10,2), " - ", ROUND(comb!D10,2),  ")", IF(OR(comb!C10 &gt;1, comb!D10 &lt;1), "*", " ") )</f>
+        <v xml:space="preserve">1.01 (0.79 - 1.29) </v>
+      </c>
+      <c r="G6" s="9" t="str">
+        <f>_xlfn.CONCAT(ROUND(comb!B11, 2), " (", ROUND(comb!C11,2), " - ", ROUND(comb!D11,2),  ")", IF(OR(comb!C11 &gt;1, comb!D11 &lt;1), "*", " ") )</f>
+        <v xml:space="preserve">1.11 (0.68 - 1.83) </v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="8" t="str">
+        <f>_xlfn.CONCAT(ROUND(comb!B12, 2), " (", ROUND(comb!C12,2), " - ", ROUND(comb!D12,2),  ")", IF(OR(comb!C12 &gt;1, comb!D12 &lt;1), "*", " ") )</f>
+        <v>1.37 (1.26 - 1.5)*</v>
+      </c>
+      <c r="D7" s="8" t="str">
+        <f>_xlfn.CONCAT(ROUND(comb!B13, 2), " (", ROUND(comb!C13,2), " - ", ROUND(comb!D13,2),  ")", IF(OR(comb!C13 &gt;1, comb!D13 &lt;1), "*", " ") )</f>
+        <v>1.4 (1.23 - 1.6)*</v>
+      </c>
+      <c r="E7" s="8" t="str">
+        <f>_xlfn.CONCAT(ROUND(comb!B14, 2), " (", ROUND(comb!C14,2), " - ", ROUND(comb!D14,2),  ")",IF(OR(comb!C14 &gt;1, comb!D14 &lt;1), "*", " ") )</f>
+        <v>1.37 (1.2 - 1.57)*</v>
+      </c>
+      <c r="F7" s="8" t="str">
+        <f>_xlfn.CONCAT(ROUND(comb!B15, 2), " (", ROUND(comb!C15,2), " - ", ROUND(comb!D15,2),  ")", IF(OR(comb!C15 &gt;1, comb!D15 &lt;1), "*", " ") )</f>
+        <v xml:space="preserve">1.25 (0.89 - 1.75) </v>
+      </c>
+      <c r="G7" s="9" t="str">
+        <f>_xlfn.CONCAT(ROUND(comb!B16, 2), " (", ROUND(comb!C16,2), " - ", ROUND(comb!D16,2),  ")", IF(OR(comb!C16 &gt;1, comb!D16 &lt;1), "*", " ") )</f>
+        <v xml:space="preserve">0.66 (0.07 - 6.47) </v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C8" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:G3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
bugfixes to log_reg in R
</commit_message>
<xml_diff>
--- a/results/LOG_REG.xlsx
+++ b/results/LOG_REG.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tristan/Documents/Projekte/Boston Celi/1 Causal Inference/Race Interventions/mit-tmle/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08823977-07AA-764D-BB13-2E0216ADCED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D29EA4-B5EE-544C-89E9-9CB3BD2E2811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35960" yWindow="-680" windowWidth="15880" windowHeight="20500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MIMIC" sheetId="1" r:id="rId1"/>
@@ -1690,8 +1690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6EE9FD-E04A-1B49-B8E8-A06D1A48705F}">
   <dimension ref="A1:V16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1736,13 +1736,13 @@
         <v>5</v>
       </c>
       <c r="B2" s="1">
-        <v>1.1464086253903594</v>
+        <v>1.1309312901102899</v>
       </c>
       <c r="C2" s="1">
-        <v>1.0522206844645743</v>
+        <v>1.0784326442360199</v>
       </c>
       <c r="D2" s="1">
-        <v>1.2490276571954815</v>
+        <v>1.18607793415198</v>
       </c>
       <c r="E2" s="1">
         <v>1.7859781053329708E-3</v>
@@ -1764,13 +1764,13 @@
         <v>6</v>
       </c>
       <c r="B3" s="1">
-        <v>1.1501060738118938</v>
+        <v>1.06971455992771</v>
       </c>
       <c r="C3" s="1">
-        <v>1.0149126450412029</v>
+        <v>1.0058477673878301</v>
       </c>
       <c r="D3" s="1">
-        <v>1.3033082083289138</v>
+        <v>1.1379590258515</v>
       </c>
       <c r="E3" s="1">
         <v>2.8381832317266327E-2</v>
@@ -1797,13 +1797,13 @@
         <v>7</v>
       </c>
       <c r="B4" s="1">
-        <v>1.2003411110367985</v>
+        <v>0.89193697823272999</v>
       </c>
       <c r="C4" s="1">
-        <v>1.0514690835535825</v>
+        <v>0.70935976294855496</v>
       </c>
       <c r="D4" s="1">
-        <v>1.3702911529986346</v>
+        <v>1.1142677914804699</v>
       </c>
       <c r="E4" s="1">
         <v>6.8753688959064686E-3</v>
@@ -1830,13 +1830,13 @@
         <v>8</v>
       </c>
       <c r="B5" s="1">
-        <v>0.8733928506005515</v>
+        <v>1.59311166392922</v>
       </c>
       <c r="C5" s="1">
-        <v>0.64674458637657894</v>
+        <v>0.65366884681395299</v>
       </c>
       <c r="D5" s="1">
-        <v>1.1794688158951114</v>
+        <v>3.61111377299695</v>
       </c>
       <c r="E5" s="1">
         <v>0.377170179292666</v>
@@ -1863,13 +1863,13 @@
         <v>9</v>
       </c>
       <c r="B6" s="1">
-        <v>1.6450518443358078</v>
+        <v>1.2683009701883401</v>
       </c>
       <c r="C6" s="1">
-        <v>0.68560235521592516</v>
+        <v>1.17149885738621</v>
       </c>
       <c r="D6" s="1">
-        <v>3.9471795129705285</v>
+        <v>1.37305232294473</v>
       </c>
       <c r="E6" s="1">
         <v>0.26498056312302865</v>
@@ -1896,13 +1896,13 @@
         <v>10</v>
       </c>
       <c r="B7" s="1">
-        <v>0.71376953055250036</v>
+        <v>0.66265520206337003</v>
       </c>
       <c r="C7" s="1">
-        <v>0.62208784789881533</v>
+        <v>0.61595434030856799</v>
       </c>
       <c r="D7" s="1">
-        <v>0.81896302020032907</v>
+        <v>0.71325985992333396</v>
       </c>
       <c r="E7" s="1">
         <v>1.5304637777699025E-6</v>
@@ -1913,13 +1913,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>0.51535031698170841</v>
+        <v>0.61775214777807597</v>
       </c>
       <c r="C8" s="1">
-        <v>0.36466030359707302</v>
+        <v>0.54252851658903301</v>
       </c>
       <c r="D8" s="1">
-        <v>0.72831055805460876</v>
+        <v>0.70487035467919001</v>
       </c>
       <c r="E8" s="1">
         <v>1.7235425397791034E-4</v>
@@ -1930,13 +1930,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="1">
-        <v>0.59841644836381103</v>
+        <v>0.98900302050492594</v>
       </c>
       <c r="C9" s="1">
-        <v>0.4906833997111138</v>
+        <v>0.83191932389569201</v>
       </c>
       <c r="D9" s="1">
-        <v>0.72980305810872692</v>
+        <v>1.17855685649418</v>
       </c>
       <c r="E9" s="1">
         <v>3.9732785637163997E-7</v>
@@ -1947,13 +1947,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="1">
-        <v>1.0103488835969268</v>
+        <v>0.98128666703356404</v>
       </c>
       <c r="C10" s="1">
-        <v>0.78990668945638298</v>
+        <v>0.63917838094839496</v>
       </c>
       <c r="D10" s="1">
-        <v>1.2923106997461664</v>
+        <v>1.5046406396865599</v>
       </c>
       <c r="E10" s="1">
         <v>0.93465951555910753</v>
@@ -1964,13 +1964,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="1">
-        <v>1.1148168957222486</v>
+        <v>0.60727253559376304</v>
       </c>
       <c r="C11" s="1">
-        <v>0.68086442488967502</v>
+        <v>0.54724986293529398</v>
       </c>
       <c r="D11" s="1">
-        <v>1.8253512234673925</v>
+        <v>0.67449379385817099</v>
       </c>
       <c r="E11" s="1">
         <v>0.66571592446898264</v>
@@ -1981,13 +1981,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>1.374269158888465</v>
+        <v>1.2111381788053199</v>
       </c>
       <c r="C12" s="1">
-        <v>1.2557498354121508</v>
+        <v>1.1541079907199501</v>
       </c>
       <c r="D12" s="1">
-        <v>1.5039744922221274</v>
+        <v>1.2710907051537099</v>
       </c>
       <c r="E12" s="1">
         <v>4.8813356808069523E-12</v>
@@ -1998,13 +1998,13 @@
         <v>6</v>
       </c>
       <c r="B13" s="1">
-        <v>1.4003722921047703</v>
+        <v>1.19097545971218</v>
       </c>
       <c r="C13" s="1">
-        <v>1.2260204915367277</v>
+        <v>1.1191303678253299</v>
       </c>
       <c r="D13" s="1">
-        <v>1.5995185806696786</v>
+        <v>1.2678394873944101</v>
       </c>
       <c r="E13" s="1">
         <v>6.9167180514873738E-7</v>
@@ -2015,13 +2015,13 @@
         <v>7</v>
       </c>
       <c r="B14" s="1">
-        <v>1.3694723678586598</v>
+        <v>1.1381097525930399</v>
       </c>
       <c r="C14" s="1">
-        <v>1.1983280705820289</v>
+        <v>0.874616621820826</v>
       </c>
       <c r="D14" s="1">
-        <v>1.5650593625980023</v>
+        <v>1.46920329728302</v>
       </c>
       <c r="E14" s="1">
         <v>3.9071432244698876E-6</v>
@@ -2032,13 +2032,13 @@
         <v>8</v>
       </c>
       <c r="B15" s="1">
-        <v>1.251969416989801</v>
+        <v>0.63663881685109602</v>
       </c>
       <c r="C15" s="1">
-        <v>0.89492485565891888</v>
+        <v>3.0314468484417701E-2</v>
       </c>
       <c r="D15" s="1">
-        <v>1.7514626073534523</v>
+        <v>4.6221487017009402</v>
       </c>
       <c r="E15" s="1">
         <v>0.18956365188063862</v>
@@ -2049,13 +2049,13 @@
         <v>9</v>
       </c>
       <c r="B16" s="1">
-        <v>0.66073162185445655</v>
+        <v>1.24999772139442</v>
       </c>
       <c r="C16" s="1">
-        <v>6.7452298291336768E-2</v>
+        <v>1.1540615675438199</v>
       </c>
       <c r="D16" s="1">
-        <v>6.4722224027537836</v>
+        <v>1.35374559920814</v>
       </c>
       <c r="E16" s="1">
         <v>0.72188722968054342</v>
@@ -2303,7 +2303,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35A21450-980D-7A4C-82EA-70868119DA27}">
   <dimension ref="A3:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="196" workbookViewId="0">
+    <sheetView zoomScale="196" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:G7"/>
     </sheetView>
   </sheetViews>
@@ -2362,23 +2362,23 @@
       </c>
       <c r="C5" s="8" t="str">
         <f>_xlfn.CONCAT(ROUND(comb!B2, 2), " (", ROUND(comb!C2,2), " - ", ROUND(comb!D2,2),  ")", IF(OR(comb!C2 &gt;1, comb!D2 &lt;1), "*", " ") )</f>
-        <v>1.15 (1.05 - 1.25)*</v>
+        <v>1.13 (1.08 - 1.19)*</v>
       </c>
       <c r="D5" s="8" t="str">
         <f>_xlfn.CONCAT(ROUND(comb!B3, 2), " (", ROUND(comb!C3,2), " - ", ROUND(comb!D3,2),  ")", IF(OR(comb!C3 &gt;1, comb!D3 &lt;1), "*", " ") )</f>
-        <v>1.15 (1.01 - 1.3)*</v>
+        <v>1.07 (1.01 - 1.14)*</v>
       </c>
       <c r="E5" s="8" t="str">
         <f>_xlfn.CONCAT(ROUND(comb!B4, 2), " (", ROUND(comb!C4,2), " - ", ROUND(comb!D4,2),  ")", IF(OR(comb!C4 &gt;1, comb!D4 &lt;1), "*", " ") )</f>
-        <v>1.2 (1.05 - 1.37)*</v>
+        <v xml:space="preserve">0.89 (0.71 - 1.11) </v>
       </c>
       <c r="F5" s="8" t="str">
         <f>_xlfn.CONCAT(ROUND(comb!B5, 2), " (", ROUND(comb!C5,2), " - ", ROUND(comb!D5,2),  ")", IF(OR(comb!C5 &gt;1, comb!D5 &lt;1), "*", " ") )</f>
-        <v xml:space="preserve">0.87 (0.65 - 1.18) </v>
+        <v xml:space="preserve">1.59 (0.65 - 3.61) </v>
       </c>
       <c r="G5" s="9" t="str">
         <f>_xlfn.CONCAT(ROUND(comb!B6, 2), " (", ROUND(comb!C6,2), " - ", ROUND(comb!D6,2),  ")", IF(OR(comb!C6 &gt;1, comb!D6 &lt;1), "*", " ") )</f>
-        <v xml:space="preserve">1.65 (0.69 - 3.95) </v>
+        <v>1.27 (1.17 - 1.37)*</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2390,23 +2390,23 @@
       </c>
       <c r="C6" s="8" t="str">
         <f>_xlfn.CONCAT(ROUND(comb!B7, 2), " (", ROUND(comb!C7,2), " - ", ROUND(comb!D7,2),  ")", IF(OR(comb!C7 &gt;1, comb!D7 &lt;1), "*", " ") )</f>
-        <v>0.71 (0.62 - 0.82)*</v>
+        <v>0.66 (0.62 - 0.71)*</v>
       </c>
       <c r="D6" s="8" t="str">
         <f>_xlfn.CONCAT(ROUND(comb!B8, 2), " (", ROUND(comb!C8,2), " - ", ROUND(comb!D8,2),  ")", IF(OR(comb!C8 &gt;1, comb!D8 &lt;1), "*", " ") )</f>
-        <v>0.52 (0.36 - 0.73)*</v>
+        <v>0.62 (0.54 - 0.7)*</v>
       </c>
       <c r="E6" s="8" t="str">
         <f>_xlfn.CONCAT(ROUND(comb!B9, 2), " (", ROUND(comb!C9,2), " - ", ROUND(comb!D9,2),  ")", IF(OR(comb!C9 &gt;1, comb!D9 &lt;1), "*", " ") )</f>
-        <v>0.6 (0.49 - 0.73)*</v>
+        <v xml:space="preserve">0.99 (0.83 - 1.18) </v>
       </c>
       <c r="F6" s="8" t="str">
         <f>_xlfn.CONCAT(ROUND(comb!B10, 2), " (", ROUND(comb!C10,2), " - ", ROUND(comb!D10,2),  ")", IF(OR(comb!C10 &gt;1, comb!D10 &lt;1), "*", " ") )</f>
-        <v xml:space="preserve">1.01 (0.79 - 1.29) </v>
+        <v xml:space="preserve">0.98 (0.64 - 1.5) </v>
       </c>
       <c r="G6" s="9" t="str">
         <f>_xlfn.CONCAT(ROUND(comb!B11, 2), " (", ROUND(comb!C11,2), " - ", ROUND(comb!D11,2),  ")", IF(OR(comb!C11 &gt;1, comb!D11 &lt;1), "*", " ") )</f>
-        <v xml:space="preserve">1.11 (0.68 - 1.83) </v>
+        <v>0.61 (0.55 - 0.67)*</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2418,23 +2418,23 @@
       </c>
       <c r="C7" s="8" t="str">
         <f>_xlfn.CONCAT(ROUND(comb!B12, 2), " (", ROUND(comb!C12,2), " - ", ROUND(comb!D12,2),  ")", IF(OR(comb!C12 &gt;1, comb!D12 &lt;1), "*", " ") )</f>
-        <v>1.37 (1.26 - 1.5)*</v>
+        <v>1.21 (1.15 - 1.27)*</v>
       </c>
       <c r="D7" s="8" t="str">
         <f>_xlfn.CONCAT(ROUND(comb!B13, 2), " (", ROUND(comb!C13,2), " - ", ROUND(comb!D13,2),  ")", IF(OR(comb!C13 &gt;1, comb!D13 &lt;1), "*", " ") )</f>
-        <v>1.4 (1.23 - 1.6)*</v>
+        <v>1.19 (1.12 - 1.27)*</v>
       </c>
       <c r="E7" s="8" t="str">
         <f>_xlfn.CONCAT(ROUND(comb!B14, 2), " (", ROUND(comb!C14,2), " - ", ROUND(comb!D14,2),  ")",IF(OR(comb!C14 &gt;1, comb!D14 &lt;1), "*", " ") )</f>
-        <v>1.37 (1.2 - 1.57)*</v>
+        <v xml:space="preserve">1.14 (0.87 - 1.47) </v>
       </c>
       <c r="F7" s="8" t="str">
         <f>_xlfn.CONCAT(ROUND(comb!B15, 2), " (", ROUND(comb!C15,2), " - ", ROUND(comb!D15,2),  ")", IF(OR(comb!C15 &gt;1, comb!D15 &lt;1), "*", " ") )</f>
-        <v xml:space="preserve">1.25 (0.89 - 1.75) </v>
+        <v xml:space="preserve">0.64 (0.03 - 4.62) </v>
       </c>
       <c r="G7" s="9" t="str">
         <f>_xlfn.CONCAT(ROUND(comb!B16, 2), " (", ROUND(comb!C16,2), " - ", ROUND(comb!D16,2),  ")", IF(OR(comb!C16 &gt;1, comb!D16 &lt;1), "*", " ") )</f>
-        <v xml:space="preserve">0.66 (0.07 - 6.47) </v>
+        <v>1.25 (1.15 - 1.35)*</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>